<commit_message>
RU: modified entregables_fechas y template_documentacion_sprint_5
</commit_message>
<xml_diff>
--- a/RUBRICAS_Y_PLANTILLAS/entregables_fechas.xlsx
+++ b/RUBRICAS_Y_PLANTILLAS/entregables_fechas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\Repo\CICLO-III\RUBRICAS_Y_PLANTILLAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B9A431-282C-4A4A-9654-372DD6AD7D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B540E84-388B-4130-AA5E-06AA0FDFB5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,61 +411,6 @@
         <color theme="1"/>
         <rFont val="Arial"/>
       </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Documento actualizado en formato .pdf con las especificaciones y configuraciones del servidor virtual en la nube sobre el que se realizará el despliegue. Además, el documento debe contener el Enlace/URL de la aplicación desplegada.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Implementación final y funcional de la aplicación.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Manual de Usuario en formato .pdf.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
       <t xml:space="preserve">1. </t>
     </r>
     <r>
@@ -521,6 +466,43 @@
   </si>
   <si>
     <t>2021-10-25, 23:59</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Documento actualizado en formato .pdf con la descripción de los requerimientos y el proceso de despliegue de la aplicación en una Plataforma como Servicio (PaaS). Además, el documento debe contener el Enlace/URL de la aplicación desplegada.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> Implementación final y funcional de la aplicación.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1077,8 +1059,8 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1156,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -1210,10 +1192,10 @@
         <v>9</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1249,10 +1231,10 @@
         <v>11</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1288,10 +1270,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1321,16 +1303,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>

</xml_diff>